<commit_message>
test for attached file and Word
</commit_message>
<xml_diff>
--- a/Documentation/(Test) Upgrade Release Notes.xlsx
+++ b/Documentation/(Test) Upgrade Release Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixin.li\Desktop\N4 upgrade\DCB\GitHub - DCB\ACNKristinLi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9828A5-9F02-451A-999A-20B3219ADB03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E864DF0-A002-47DF-BA28-11614B3E7761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24105" windowHeight="15510" tabRatio="665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Pre-Cutover Items" sheetId="1" r:id="rId1"/>
@@ -3288,8 +3288,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>1019175</xdr:colOff>
-          <xdr:row>17</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4346,11 +4346,11 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4815,11 +4815,11 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5924,8 +5924,8 @@
               <to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>1019175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>342900</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -9282,18 +9282,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9315,6 +9315,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CADD70B2-10FF-4224-B7A3-E4E043449098}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9328,12 +9336,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update (Test) Upgrade Release Notes.xlsx
test
</commit_message>
<xml_diff>
--- a/Documentation/(Test) Upgrade Release Notes.xlsx
+++ b/Documentation/(Test) Upgrade Release Notes.xlsx
@@ -5,28 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixin.li\Desktop\N4 upgrade\DCB\GitHub - DCB\ACNKristinLi\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lyon.yujun.lai\Documents\GitHub\ACNKristinLi\DomainRep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E864DF0-A002-47DF-BA28-11614B3E7761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9204D6-C002-4131-AB12-95E252A0159A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="24105" windowHeight="15510" tabRatio="665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Pre-Cutover Items" sheetId="1" r:id="rId1"/>
     <sheet name="2. Cutover Items" sheetId="2" r:id="rId2"/>
-    <sheet name="3. Variforms" sheetId="23" r:id="rId3"/>
-    <sheet name="4. Custom Menus" sheetId="24" r:id="rId4"/>
-    <sheet name="5. General Reference" sheetId="10" r:id="rId5"/>
-    <sheet name="6. DBA Action" sheetId="9" r:id="rId6"/>
-    <sheet name="7. New Groovy Job" sheetId="25" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId3"/>
+    <sheet name="3. Variforms" sheetId="23" r:id="rId4"/>
+    <sheet name="4. Custom Menus" sheetId="24" r:id="rId5"/>
+    <sheet name="5. General Reference" sheetId="10" r:id="rId6"/>
+    <sheet name="6. DBA Action" sheetId="9" r:id="rId7"/>
+    <sheet name="7. New Groovy Job" sheetId="25" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. Cutover Items'!$B$1:$L$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'3. Variforms'!$A$2:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Custom Menus'!$A$28:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'3. Variforms'!$A$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'4. Custom Menus'!$A$28:$K$28</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4815,7 +4816,7 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6015,6 +6016,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAE1BDA-80C8-4074-B5F2-ACCDABA46FD7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="284" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
@@ -6825,7 +6839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K71"/>
   <sheetViews>
@@ -8285,7 +8299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -8576,7 +8590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -8833,7 +8847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:Q12"/>
   <sheetViews>
@@ -9282,18 +9296,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9315,14 +9329,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CADD70B2-10FF-4224-B7A3-E4E043449098}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9336,4 +9342,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test for sheet visibility
</commit_message>
<xml_diff>
--- a/Documentation/(Test) Upgrade Release Notes.xlsx
+++ b/Documentation/(Test) Upgrade Release Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixin.li\Desktop\N4 upgrade\DCB\GitHub - DCB\ACNKristinLi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC97253-CCA5-406B-A2D9-F18013B8CD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6616F3F2-91B7-489F-8DC5-CAC8924793E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="105" windowWidth="24105" windowHeight="15510" tabRatio="665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Pre-Cutover Items" sheetId="1" r:id="rId1"/>
@@ -3520,7 +3520,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3564,7 +3564,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3613,7 +3613,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3657,7 +3657,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3700,7 +3700,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3753,7 +3753,7 @@
                   <a14:compatExt spid="_x0000_s10241"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001280000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000001280000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3808,7 +3808,7 @@
                   <a14:compatExt spid="_x0000_s10242"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002280000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002280000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3863,7 +3863,7 @@
                   <a14:compatExt spid="_x0000_s10243"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003280000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003280000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3918,7 +3918,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3962,7 +3962,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4006,7 +4006,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4050,7 +4050,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6017,16 +6017,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F409FDDC-1446-4C09-B200-F83F26B971F8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="31">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="31">
         <v>123456</v>
       </c>
     </row>
@@ -9139,21 +9234,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B189D02CC4F2E4EB849E1B81E4E4439" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="540013ce737e003674d6eb05c8e71aa7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c94e8d52-508f-4203-8afe-1c5bccd7ba62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c20b3495edfcc628fa38bee0294f95a0" ns2:_="">
     <xsd:import namespace="c94e8d52-508f-4203-8afe-1c5bccd7ba62"/>
@@ -9317,31 +9397,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CADD70B2-10FF-4224-B7A3-E4E043449098}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c94e8d52-508f-4203-8afe-1c5bccd7ba62"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0A1D4F-997F-4105-B171-4ED9E5AE8D23}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9357,4 +9428,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96643455-72E5-48F7-B1B0-1EF101958494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CADD70B2-10FF-4224-B7A3-E4E043449098}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c94e8d52-508f-4203-8afe-1c5bccd7ba62"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>